<commit_message>
Added Clinical Labs Form
</commit_message>
<xml_diff>
--- a/Current Patients/12345/DataBases/Data/12345_Alertness_Source.xlsx
+++ b/Current Patients/12345/DataBases/Data/12345_Alertness_Source.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -672,10 +672,52 @@
           <t>23424</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
           <t>sdfsdfsff</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>54654</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>07/20/2020</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>asdasda</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
         </is>
       </c>
     </row>

</xml_diff>